<commit_message>
JS8 - tugas 1 (implement import in kategori, level, supplier, user)
</commit_message>
<xml_diff>
--- a/MINGGU_8/PWL_POS/public/template_barang.xlsx
+++ b/MINGGU_8/PWL_POS/public/template_barang.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\WebLanjut\MINGGU_8\PWL_POS\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{827AD680-700C-4889-8B89-755B8672E88E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A48073A-EC7F-4B7E-9A05-372D5CCE276C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{082F3336-5ADF-47FE-893D-DF8B093DDEEA}"/>
+    <workbookView xWindow="4392" yWindow="3360" windowWidth="17280" windowHeight="8880" xr2:uid="{082F3336-5ADF-47FE-893D-DF8B093DDEEA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -76,7 +76,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -90,6 +90,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -99,7 +107,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -107,12 +115,34 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -430,7 +460,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -442,104 +472,104 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2">
+      <c r="A2" s="2">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="1">
         <v>8000</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="1">
         <v>10000</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3">
+      <c r="A3" s="2">
         <v>16</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="1">
         <v>250000</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="1">
         <v>300000</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4">
+      <c r="A4" s="2">
         <v>18</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="1">
         <v>70000</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="1">
         <v>9000</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5">
+      <c r="A5" s="2">
         <v>19</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="1">
         <v>14000</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="1">
         <v>15500</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6">
+      <c r="A6" s="2">
         <v>20</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="1">
         <v>30000</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="1">
         <v>35000</v>
       </c>
     </row>

</xml_diff>